<commit_message>
Generating the excel Report using the Apache-poi....
</commit_message>
<xml_diff>
--- a/Student/src/main/webapp/WEB-INF/report/StudentReport.xlsx
+++ b/Student/src/main/webapp/WEB-INF/report/StudentReport.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AAAAAA" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -64,12 +64,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,27 +373,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>